<commit_message>
Agregamos el tp3 MS Excel finalizado.
</commit_message>
<xml_diff>
--- a/trabajos practicos/excel/Excel2024-TP2.xlsx
+++ b/trabajos practicos/excel/Excel2024-TP2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\VSCode Projects\microsoftoffice\microsoftoffice\trabajos practicos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FA2E22-E49F-47EC-A342-AD680DC85CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D4B215-FA67-493F-A67B-18848DB60008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9722A28A-0412-4DEA-A2B3-E379A2CD8163}"/>
   </bookViews>
@@ -304,9 +304,6 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -324,6 +321,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B521B125-CD75-4FAE-8EFD-6745A14119B6}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,18 +705,18 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -731,435 +731,435 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>894</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>27553</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <f t="shared" ref="D5:D15" ca="1" si="0">DATEDIF(C5, TODAY(), "Y")</f>
         <v>48</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>75.599999999999994</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <v>79.400000000000006</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="6">
         <f t="shared" ref="G5:G15" si="1">(F5-E5)/E5</f>
         <v>5.0264550264550421E-2</v>
       </c>
-      <c r="H5" s="8" t="str">
+      <c r="H5" s="7" t="str">
         <f t="shared" ref="H5:H15" si="2">IF(G5&gt;0, "Controlar", "")</f>
         <v>Controlar</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>2561</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>31138</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>67.900000000000006</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>65.099999999999994</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>-4.1237113402062021E-2</v>
       </c>
-      <c r="H6" s="8" t="str">
+      <c r="H6" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>4712</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>21120</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>99.12</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>85.4</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>-0.13841807909604517</v>
       </c>
-      <c r="H7" s="8" t="str">
+      <c r="H7" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>135</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>29640</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>78.7</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>74.400000000000006</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>-5.463786531130873E-2</v>
       </c>
-      <c r="H8" s="8" t="str">
+      <c r="H8" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>1784</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>34862</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>98.2</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>102</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>3.8696537678207708E-2</v>
       </c>
-      <c r="H9" s="8" t="str">
+      <c r="H9" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>1235</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>29184</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>75.8</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <v>77.900000000000006</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <f t="shared" si="1"/>
         <v>2.7704485488126762E-2</v>
       </c>
-      <c r="H10" s="8" t="str">
+      <c r="H10" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>6841</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>33584</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>32</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>88.35</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <v>105.4</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>0.19298245614035101</v>
       </c>
-      <c r="H11" s="8" t="str">
+      <c r="H11" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>3487</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>29917</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>95.26</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <v>103.4</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>8.5450346420323328E-2</v>
       </c>
-      <c r="H12" s="8" t="str">
+      <c r="H12" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>4898</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>20933</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>84.8</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <v>80.099999999999994</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>-5.5424528301886829E-2</v>
       </c>
-      <c r="H13" s="8" t="str">
+      <c r="H13" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>758</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>21106</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>85.22</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <v>88.6</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <f t="shared" si="1"/>
         <v>3.9662051161699081E-2</v>
       </c>
-      <c r="H14" s="8" t="str">
+      <c r="H14" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>1123</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>27730</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>85.6</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <v>92.4</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <f t="shared" si="1"/>
         <v>7.9439252336448732E-2</v>
       </c>
-      <c r="H15" s="8" t="str">
+      <c r="H15" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="4"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5">
         <f>AVERAGE(E5:E15)</f>
         <v>84.959090909090904</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f>AVERAGE(F5:F15)</f>
         <v>86.736363636363635</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
         <f>COUNTBLANK(J5:J15)</f>
         <v>3</v>
       </c>
@@ -1177,12 +1177,12 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="13">
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="12">
         <f>COUNT(A5:A15)</f>
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Terminamos los 5 tp de MS Excel.
</commit_message>
<xml_diff>
--- a/trabajos practicos/excel/Excel2024-TP2.xlsx
+++ b/trabajos practicos/excel/Excel2024-TP2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\VSCode Projects\microsoftoffice\microsoftoffice\trabajos practicos\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D4B215-FA67-493F-A67B-18848DB60008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423D721F-01E0-4447-9E96-E73ED1CC2C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9722A28A-0412-4DEA-A2B3-E379A2CD8163}"/>
+    <workbookView xWindow="75" yWindow="105" windowWidth="16605" windowHeight="15495" xr2:uid="{9722A28A-0412-4DEA-A2B3-E379A2CD8163}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -309,13 +309,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -323,6 +319,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B521B125-CD75-4FAE-8EFD-6745A14119B6}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,18 +705,18 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -776,21 +776,21 @@
         <f t="shared" ref="D5:D15" ca="1" si="0">DATEDIF(C5, TODAY(), "Y")</f>
         <v>48</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="12">
         <v>75.599999999999994</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="12">
         <v>79.400000000000006</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <f t="shared" ref="G5:G15" si="1">(F5-E5)/E5</f>
         <v>5.0264550264550421E-2</v>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="6" t="str">
         <f t="shared" ref="H5:H15" si="2">IF(G5&gt;0, "Controlar", "")</f>
         <v>Controlar</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -811,21 +811,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>38</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="12">
         <v>67.900000000000006</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="12">
         <v>65.099999999999994</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>-4.1237113402062021E-2</v>
       </c>
-      <c r="H6" s="7" t="str">
+      <c r="H6" s="6" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J6" s="3"/>
@@ -844,21 +844,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="12">
         <v>99.12</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="12">
         <v>85.4</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>-0.13841807909604517</v>
       </c>
-      <c r="H7" s="7" t="str">
+      <c r="H7" s="6" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -879,21 +879,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="12">
         <v>78.7</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="12">
         <v>74.400000000000006</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>-5.463786531130873E-2</v>
       </c>
-      <c r="H8" s="7" t="str">
+      <c r="H8" s="6" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -914,21 +914,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>28</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="12">
         <v>98.2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="13">
         <v>102</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>3.8696537678207708E-2</v>
       </c>
-      <c r="H9" s="7" t="str">
+      <c r="H9" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="3"/>
@@ -947,21 +947,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>44</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="12">
         <v>75.8</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="12">
         <v>77.900000000000006</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>2.7704485488126762E-2</v>
       </c>
-      <c r="H10" s="7" t="str">
+      <c r="H10" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>22</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -982,21 +982,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>32</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="12">
         <v>88.35</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="12">
         <v>105.4</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>0.19298245614035101</v>
       </c>
-      <c r="H11" s="7" t="str">
+      <c r="H11" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -1017,21 +1017,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="12">
         <v>95.26</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="12">
         <v>103.4</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>8.5450346420323328E-2</v>
       </c>
-      <c r="H12" s="7" t="str">
+      <c r="H12" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -1052,21 +1052,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="12">
         <v>84.8</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="12">
         <v>80.099999999999994</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>-5.5424528301886829E-2</v>
       </c>
-      <c r="H13" s="7" t="str">
+      <c r="H13" s="6" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="3" t="s">
@@ -1087,21 +1087,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>66</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="12">
         <v>85.22</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="12">
         <v>88.6</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>3.9662051161699081E-2</v>
       </c>
-      <c r="H14" s="7" t="str">
+      <c r="H14" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>23</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -1122,21 +1122,21 @@
         <f t="shared" ca="1" si="0"/>
         <v>48</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="12">
         <v>85.6</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="12">
         <v>92.4</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>7.9439252336448732E-2</v>
       </c>
-      <c r="H15" s="7" t="str">
+      <c r="H15" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Controlar</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="J15" s="3"/>
@@ -1148,11 +1148,11 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="5">
+      <c r="E16" s="12">
         <f>AVERAGE(E5:E15)</f>
         <v>84.959090909090904</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="12">
         <f>AVERAGE(F5:F15)</f>
         <v>86.736363636363635</v>
       </c>
@@ -1177,12 +1177,12 @@
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10">
         <f>COUNT(A5:A15)</f>
         <v>11</v>
       </c>

</xml_diff>